<commit_message>
Added new GA 3.2 prototype
Added "Course Sections"
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Class Schedule" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,16 +17,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -37,7 +34,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -45,20 +42,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -434,410 +425,301 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
         <is>
           <t>Monday</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Tuesday</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Wednesday</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Thursday</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Friday</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Saturday</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" t="inlineStr">
         <is>
           <t>07:00</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" t="inlineStr">
         <is>
           <t>07:30</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" t="inlineStr">
         <is>
           <t>08:00</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>CS13 - CS101 (Room 1)</t>
+        </is>
+      </c>
+      <c r="E4" s="1" t="inlineStr">
+        <is>
+          <t>CS13 - CS101 (Room 1)</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" t="inlineStr">
         <is>
           <t>08:30</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" t="inlineStr">
         <is>
           <t>09:00</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>CS13 - CS102 (Room 1)</t>
+        </is>
+      </c>
+      <c r="F6" s="1" t="inlineStr">
+        <is>
+          <t>CS13 - CS102 (Room 1)</t>
+        </is>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" t="inlineStr">
         <is>
           <t>09:30</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
+      <c r="A8" t="inlineStr">
         <is>
           <t>10:00</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>CS101 (CB 224)</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>CS12 - CS101 (Room 1)</t>
+        </is>
+      </c>
+      <c r="E8" s="1" t="inlineStr">
+        <is>
+          <t>CS12 - CS101 (Room 1)</t>
+        </is>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
+      <c r="A9" t="inlineStr">
         <is>
           <t>10:30</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
+      <c r="A10" t="inlineStr">
         <is>
           <t>11:00</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
+      <c r="D10" s="1" t="inlineStr">
+        <is>
+          <t>CS12 - CS103 (Room 2)</t>
+        </is>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
+      <c r="A11" t="inlineStr">
         <is>
           <t>11:30</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
+      <c r="A12" t="inlineStr">
         <is>
           <t>12:00</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
+      <c r="A13" t="inlineStr">
         <is>
           <t>12:30</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-      <c r="G13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="inlineStr">
+      <c r="A14" t="inlineStr">
         <is>
           <t>13:00</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>CS102 (CB 226)</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr"/>
-      <c r="E14" t="inlineStr"/>
-      <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>CS11 - CS102 (Room 3)</t>
+        </is>
+      </c>
+      <c r="F14" s="1" t="inlineStr">
+        <is>
+          <t>CS11 - CS102 (Room 3)</t>
+        </is>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="inlineStr">
+      <c r="A15" t="inlineStr">
         <is>
           <t>13:30</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr"/>
-      <c r="G15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
+      <c r="A16" t="inlineStr">
         <is>
           <t>14:00</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr"/>
-      <c r="G16" t="inlineStr"/>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="inlineStr">
+      <c r="A17" t="inlineStr">
         <is>
           <t>14:30</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr"/>
-      <c r="G17" t="inlineStr"/>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="inlineStr">
+      <c r="A18" t="inlineStr">
         <is>
           <t>15:00</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="inlineStr">
+      <c r="A19" t="inlineStr">
         <is>
           <t>15:30</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="inlineStr">
+      <c r="A20" t="inlineStr">
         <is>
           <t>16:00</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
+      <c r="D20" s="1" t="inlineStr">
+        <is>
+          <t>CS13 - CS103 (Room 4)</t>
+        </is>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="inlineStr">
+      <c r="A21" t="inlineStr">
         <is>
           <t>16:30</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="inlineStr">
+      <c r="A22" t="inlineStr">
         <is>
           <t>17:00</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr"/>
-      <c r="D22" t="inlineStr"/>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="inlineStr">
+      <c r="A23" t="inlineStr">
         <is>
           <t>17:30</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr"/>
-      <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="inlineStr">
+      <c r="A24" t="inlineStr">
         <is>
           <t>18:00</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="inlineStr">
+      <c r="A25" t="inlineStr">
         <is>
           <t>18:30</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr"/>
-      <c r="C25" t="inlineStr"/>
-      <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr"/>
-      <c r="G25" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="inlineStr">
+      <c r="A26" t="inlineStr">
         <is>
           <t>19:00</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr"/>
-      <c r="C26" t="inlineStr"/>
-      <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
-      <c r="F26" t="inlineStr"/>
-      <c r="G26" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="inlineStr">
+      <c r="A27" t="inlineStr">
         <is>
           <t>19:30</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
-      <c r="F27" t="inlineStr"/>
-      <c r="G27" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="inlineStr">
+      <c r="A28" t="inlineStr">
         <is>
           <t>20:00</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr"/>
-      <c r="G28" t="inlineStr"/>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="inlineStr">
+      <c r="A29" t="inlineStr">
         <is>
           <t>20:30</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr"/>
-      <c r="C29" t="inlineStr"/>
-      <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr"/>
-      <c r="G29" t="inlineStr"/>
     </row>
   </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="D20:D29"/>
+    <mergeCell ref="F6:F11"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="D10:D19"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="C6:C11"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="C14:C19"/>
+    <mergeCell ref="F14:F19"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>